<commit_message>
Filling sample allocation template.
</commit_message>
<xml_diff>
--- a/data-raw/FilledAllocationTemplate.xlsx
+++ b/data-raw/FilledAllocationTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/IEATools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3167F63-4EEF-BC4D-8AF7-DEEFA8173791}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F6E788-7AFB-184A-86F8-16F209B51982}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="34040" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7073" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7077" uniqueCount="109">
   <si>
     <t>Country</t>
   </si>
@@ -709,10 +709,10 @@
   <dimension ref="A1:O691"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="13" ySplit="1" topLeftCell="N121" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="13" ySplit="1" topLeftCell="N138" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J154" sqref="J154"/>
+      <selection pane="bottomRight" activeCell="I169" sqref="I169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6787,6 +6787,12 @@
       <c r="H159" t="s">
         <v>55</v>
       </c>
+      <c r="I159" t="s">
+        <v>105</v>
+      </c>
+      <c r="J159" t="s">
+        <v>106</v>
+      </c>
       <c r="K159" t="s">
         <v>54</v>
       </c>
@@ -6964,6 +6970,12 @@
       </c>
       <c r="H164" t="s">
         <v>56</v>
+      </c>
+      <c r="I164" t="s">
+        <v>105</v>
+      </c>
+      <c r="J164" t="s">
+        <v>106</v>
       </c>
       <c r="K164" t="s">
         <v>54</v>

</xml_diff>